<commit_message>
Sync evaluation-by-extraction.py and evaluation-by-generation.py: exception handling!
</commit_message>
<xml_diff>
--- a/evaluation/WN18RR/evaluation-by-extraction-100@1.xlsx
+++ b/evaluation/WN18RR/evaluation-by-extraction-100@1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,95 +436,173 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>model_id</t>
+          <t>type</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>precision_mean</t>
+          <t>model</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>recall_mean</t>
+          <t>prec_mean</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>f1_score_mean</t>
+          <t>rec_mean</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>count</t>
+          <t>f1_mean</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>valid_count</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>invalid_count</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>JSON range error</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>JSON format error</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>JSON key error</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Llama-2-13b-chat-hf</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>0.131468253968254</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>0.1631349206349206</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0.1398015873015873</v>
       </c>
-      <c r="E2" t="n">
-        <v>100</v>
+      <c r="F2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Llama-2-70b-chat-hf</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>0.2290119047619047</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>0.2525833333333333</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.2329404761904762</v>
       </c>
-      <c r="E3" t="n">
-        <v>100</v>
+      <c r="F3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Llama-2-7b-chat-hf</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>0.02805555555555555</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>0.0325</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.02916666666666666</v>
       </c>
-      <c r="E4" t="n">
-        <v>100</v>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Llama-3-70b-chat-hf</t>
         </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.78495670995671</v>
       </c>
       <c r="C5" t="n">
         <v>0.78495670995671</v>
@@ -533,17 +611,34 @@
         <v>0.78495670995671</v>
       </c>
       <c r="E5" t="n">
+        <v>0.78495670995671</v>
+      </c>
+      <c r="F5" t="n">
         <v>55</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>Llama-3-8b-chat-hf</t>
         </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.450547619047619</v>
       </c>
       <c r="C6" t="n">
         <v>0.450547619047619</v>
@@ -552,36 +647,70 @@
         <v>0.450547619047619</v>
       </c>
       <c r="E6" t="n">
-        <v>100</v>
+        <v>0.450547619047619</v>
+      </c>
+      <c r="F6" t="n">
+        <v>100</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Meta-Llama-3-70B-Instruct-Lite</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>0.5086944444444444</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>0.5166944444444445</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.5100277777777777</v>
       </c>
-      <c r="E7" t="n">
-        <v>100</v>
+      <c r="F7" t="n">
+        <v>100</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Meta-Llama-3-70B-Instruct-Turbo</t>
         </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.782531746031746</v>
       </c>
       <c r="C8" t="n">
         <v>0.782531746031746</v>
@@ -590,36 +719,70 @@
         <v>0.782531746031746</v>
       </c>
       <c r="E8" t="n">
-        <v>100</v>
+        <v>0.782531746031746</v>
+      </c>
+      <c r="F8" t="n">
+        <v>100</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>Meta-Llama-3-8B-Instruct-Lite</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>0.2702579365079365</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>0.2769246031746032</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>0.2719246031746032</v>
       </c>
-      <c r="E9" t="n">
-        <v>100</v>
+      <c r="F9" t="n">
+        <v>100</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>Meta-Llama-3-8B-Instruct-Turbo</t>
         </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.4093809523809523</v>
       </c>
       <c r="C10" t="n">
         <v>0.4093809523809523</v>
@@ -628,17 +791,34 @@
         <v>0.4093809523809523</v>
       </c>
       <c r="E10" t="n">
-        <v>100</v>
+        <v>0.4093809523809523</v>
+      </c>
+      <c r="F10" t="n">
+        <v>100</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>Meta-Llama-3.1-405B-Instruct-Turbo</t>
         </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0.8140317460317461</v>
       </c>
       <c r="C11" t="n">
         <v>0.8140317460317461</v>
@@ -647,45 +827,94 @@
         <v>0.8140317460317461</v>
       </c>
       <c r="E11" t="n">
-        <v>100</v>
+        <v>0.8140317460317461</v>
+      </c>
+      <c r="F11" t="n">
+        <v>100</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>Meta-Llama-3.1-70B-Instruct-Turbo</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>0.6844761904761905</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>0.6841587301587302</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>0.684297619047619</v>
       </c>
-      <c r="E12" t="n">
-        <v>100</v>
+      <c r="F12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>Meta-Llama-3.1-8B-Instruct-Turbo</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>0.4666666666666666</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>0.4553571428571428</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>0.4583030303030303</v>
       </c>
-      <c r="E13" t="n">
-        <v>100</v>
+      <c r="F13" t="n">
+        <v>100</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>